<commit_message>
swapped PT1000_1 and _2 in X7 of RI versions
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/connectors.xlsx
+++ b/docs/Manual/source/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="48"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -1238,6 +1238,15 @@
     <t xml:space="preserve">Analogová zem</t>
   </si>
   <si>
+    <t xml:space="preserve">PT1000_2+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vstup pro 2. PT1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT1000_2-</t>
+  </si>
+  <si>
     <t xml:space="preserve">PT1000_1+</t>
   </si>
   <si>
@@ -1245,15 +1254,6 @@
   </si>
   <si>
     <t xml:space="preserve">PT1000_1-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT1000_2+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vstup pro 2. PT1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT1000_2-</t>
   </si>
   <si>
     <t xml:space="preserve">DITTL1</t>
@@ -1783,7 +1783,7 @@
   </sheetPr>
   <dimension ref="A1:K148"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H59" activeCellId="0" sqref="H59"/>
     </sheetView>
   </sheetViews>
@@ -7313,7 +7313,7 @@
   </sheetPr>
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
     </sheetView>
   </sheetViews>
@@ -11940,8 +11940,8 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
added categories D-560-x/y added S-48-100/xyz-O
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/connectors.xlsx
+++ b/docs/Manual/source/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="48"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="445">
   <si>
     <t xml:space="preserve">Toto je sešit se zdrojovými tabulkami popisu konektorů TGZ/TGS v češtině. Každý list odpovídá jednomu unikátnímu typu konektoru. Jelikož se často konektory v rámci TGZ opakují (typicky ty na řídicií desce), jsou zde jen jednou. Tj. Např. IO konektor 22pin weidmuller B2CF se používá pořád dokola, je zde tedy zanesen jen jednou jako „X8_IO_22pin_B2CF“</t>
   </si>
@@ -819,6 +819,9 @@
   </si>
   <si>
     <t xml:space="preserve">0,13 ~ 2,5 mm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+B2</t>
   </si>
   <si>
     <t xml:space="preserve">+ Brzda motor 2</t>
@@ -1783,7 +1786,7 @@
   </sheetPr>
   <dimension ref="A1:K148"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H59" activeCellId="0" sqref="H59"/>
     </sheetView>
   </sheetViews>
@@ -7931,8 +7934,8 @@
   </sheetPr>
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F40" activeCellId="0" sqref="F40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7974,12 +7977,11 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="str">
-        <f aca="false">+B2</f>
-        <v>-B2</v>
+      <c r="B3" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>236</v>
@@ -7993,7 +7995,7 @@
         <v>225</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>236</v>
@@ -8007,7 +8009,7 @@
         <v>226</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>236</v>
@@ -8018,10 +8020,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>236</v>
@@ -8032,10 +8034,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>236</v>
@@ -8096,10 +8098,10 @@
         <v>115</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8107,13 +8109,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8127,7 +8129,7 @@
         <v>120</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8141,7 +8143,7 @@
         <v>111</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8155,7 +8157,7 @@
         <v>114</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -8210,10 +8212,10 @@
         <v>115</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8221,13 +8223,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8238,10 +8240,10 @@
         <v>226</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8252,10 +8254,10 @@
         <v>225</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -8310,10 +8312,10 @@
         <v>173</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8324,10 +8326,10 @@
         <v>173</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8338,10 +8340,10 @@
         <v>173</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8352,10 +8354,10 @@
         <v>119</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -8407,13 +8409,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8421,13 +8423,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -8484,7 +8486,7 @@
         <v>205</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8498,7 +8500,7 @@
         <v>208</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8512,7 +8514,7 @@
         <v>210</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8526,7 +8528,7 @@
         <v>212</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8540,7 +8542,7 @@
         <v>214</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8554,7 +8556,7 @@
         <v>216</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8622,10 +8624,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>206</v>
@@ -8636,10 +8638,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>206</v>
@@ -8650,10 +8652,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>206</v>
@@ -8664,10 +8666,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>206</v>
@@ -8678,10 +8680,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>206</v>
@@ -8692,10 +8694,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>206</v>
@@ -8706,7 +8708,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>210</v>
@@ -8720,10 +8722,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>206</v>
@@ -8734,10 +8736,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>206</v>
@@ -8795,10 +8797,10 @@
         <v>121</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8812,7 +8814,7 @@
         <v>125</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8826,7 +8828,7 @@
         <v>210</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -8883,7 +8885,7 @@
         <v>205</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8897,7 +8899,7 @@
         <v>208</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8911,7 +8913,7 @@
         <v>210</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8925,7 +8927,7 @@
         <v>212</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8939,7 +8941,7 @@
         <v>214</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8953,7 +8955,7 @@
         <v>216</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9021,10 +9023,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>206</v>
@@ -9035,10 +9037,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>206</v>
@@ -9049,10 +9051,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>206</v>
@@ -9063,10 +9065,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>206</v>
@@ -9077,10 +9079,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>206</v>
@@ -9091,10 +9093,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>206</v>
@@ -9105,10 +9107,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>206</v>
@@ -9119,10 +9121,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>206</v>
@@ -9133,7 +9135,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>210</v>
@@ -9147,10 +9149,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>206</v>
@@ -9161,10 +9163,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>206</v>
@@ -9331,13 +9333,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9345,13 +9347,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9639,10 +9641,10 @@
         <v>204</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9653,10 +9655,10 @@
         <v>207</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9664,13 +9666,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9678,13 +9680,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9741,10 +9743,10 @@
         <v>204</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9755,10 +9757,10 @@
         <v>207</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9766,13 +9768,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9780,13 +9782,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9852,10 +9854,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>123</v>
@@ -9866,10 +9868,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>123</v>
@@ -9923,13 +9925,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9937,13 +9939,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9951,13 +9953,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>210</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9965,13 +9967,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9979,13 +9981,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9993,13 +9995,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10007,13 +10009,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10021,13 +10023,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10091,10 +10093,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>112</v>
@@ -10105,10 +10107,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>112</v>
@@ -10119,10 +10121,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>112</v>
@@ -10133,10 +10135,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>112</v>
@@ -10191,13 +10193,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10205,13 +10207,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10219,13 +10221,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10233,13 +10235,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>324</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -10287,7 +10289,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>166</v>
@@ -10298,7 +10300,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>164</v>
@@ -10309,7 +10311,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>162</v>
@@ -10320,7 +10322,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>160</v>
@@ -10331,7 +10333,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>158</v>
@@ -10342,7 +10344,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>156</v>
@@ -10353,7 +10355,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>154</v>
@@ -10364,7 +10366,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>152</v>
@@ -10375,10 +10377,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10386,10 +10388,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10512,7 +10514,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>166</v>
@@ -10523,7 +10525,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>164</v>
@@ -10534,7 +10536,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>162</v>
@@ -10545,7 +10547,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>160</v>
@@ -10556,7 +10558,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>158</v>
@@ -10567,7 +10569,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>156</v>
@@ -10578,7 +10580,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>154</v>
@@ -10589,7 +10591,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>152</v>
@@ -10600,10 +10602,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10611,10 +10613,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10657,10 +10659,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>108</v>
@@ -10668,24 +10670,24 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10769,10 +10771,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>112</v>
@@ -10783,10 +10785,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>112</v>
@@ -10800,7 +10802,7 @@
         <v>115</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>112</v>
@@ -11134,7 +11136,7 @@
         <v>182</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11272,7 +11274,7 @@
         <v>183</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11314,7 +11316,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>59</v>
@@ -11323,7 +11325,7 @@
         <v>200</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11331,7 +11333,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>59</v>
@@ -11340,7 +11342,7 @@
         <v>198</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11348,7 +11350,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>192</v>
@@ -11357,7 +11359,7 @@
         <v>196</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11365,7 +11367,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>191</v>
@@ -11374,7 +11376,7 @@
         <v>194</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11425,7 +11427,7 @@
         <v>190</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11442,7 +11444,7 @@
         <v>188</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11526,7 +11528,7 @@
         <v>183</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11568,7 +11570,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>59</v>
@@ -11577,7 +11579,7 @@
         <v>200</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11585,7 +11587,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>59</v>
@@ -11594,7 +11596,7 @@
         <v>198</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11602,7 +11604,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>192</v>
@@ -11611,7 +11613,7 @@
         <v>196</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11619,7 +11621,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>191</v>
@@ -11628,7 +11630,7 @@
         <v>194</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11746,7 +11748,7 @@
         <v>183</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11788,7 +11790,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>59</v>
@@ -11797,7 +11799,7 @@
         <v>200</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11805,7 +11807,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>59</v>
@@ -11814,7 +11816,7 @@
         <v>198</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11822,7 +11824,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>192</v>
@@ -11831,7 +11833,7 @@
         <v>196</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11839,7 +11841,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>191</v>
@@ -11848,7 +11850,7 @@
         <v>194</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11940,7 +11942,7 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -11967,10 +11969,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11981,7 +11983,7 @@
         <v>126</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11989,10 +11991,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12000,10 +12002,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12011,10 +12013,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12022,10 +12024,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12033,10 +12035,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12047,7 +12049,7 @@
         <v>149</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12055,10 +12057,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12069,7 +12071,7 @@
         <v>149</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12077,10 +12079,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12091,7 +12093,7 @@
         <v>149</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12495,7 +12497,7 @@
         <v>165</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12506,7 +12508,7 @@
         <v>163</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12517,7 +12519,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12528,7 +12530,7 @@
         <v>159</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12539,7 +12541,7 @@
         <v>157</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12550,7 +12552,7 @@
         <v>155</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12561,7 +12563,7 @@
         <v>153</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12572,7 +12574,7 @@
         <v>151</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12580,10 +12582,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12591,10 +12593,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12602,10 +12604,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12613,10 +12615,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12627,7 +12629,7 @@
         <v>143</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12638,7 +12640,7 @@
         <v>141</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12649,7 +12651,7 @@
         <v>139</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12660,7 +12662,7 @@
         <v>137</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12671,7 +12673,7 @@
         <v>135</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12682,7 +12684,7 @@
         <v>133</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -12730,10 +12732,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12741,10 +12743,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12752,10 +12754,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12763,10 +12765,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12774,10 +12776,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12785,10 +12787,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12796,10 +12798,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12807,10 +12809,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -12858,10 +12860,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12869,10 +12871,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12880,10 +12882,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12891,10 +12893,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12902,10 +12904,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12916,7 +12918,7 @@
         <v>119</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12924,10 +12926,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12935,10 +12937,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12946,10 +12948,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12957,10 +12959,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13017,10 +13019,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13028,10 +13030,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13039,10 +13041,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13050,10 +13052,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13061,10 +13063,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13072,10 +13074,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13083,10 +13085,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13094,10 +13096,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
gitignore edit TGS-560-25 work (images, connectors, tables)
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/connectors.xlsx
+++ b/docs/Manual/source/tab/connectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="59"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="60"/>
   </bookViews>
   <sheets>
     <sheet name="rozcestnik" sheetId="1" state="visible" r:id="rId3"/>
@@ -68,6 +68,10 @@
     <sheet name="X6_TGS560_50_DCbus" sheetId="58" state="visible" r:id="rId60"/>
     <sheet name="X4_TGS560_24V_5pin_BCZ" sheetId="59" state="visible" r:id="rId61"/>
     <sheet name="S1_TGS560_DIP" sheetId="60" state="visible" r:id="rId62"/>
+    <sheet name="LED_TGS560" sheetId="61" state="visible" r:id="rId63"/>
+    <sheet name="X4_ACIN_4pin_TGS560_25" sheetId="62" state="visible" r:id="rId64"/>
+    <sheet name="X1_DC_6pin_TGS560_25" sheetId="63" state="visible" r:id="rId65"/>
+    <sheet name="X5_RBR_3pin_TGS560_25" sheetId="64" state="visible" r:id="rId66"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -79,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1961" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="493">
   <si>
     <t xml:space="preserve">Toto je sešit se zdrojovými tabulkami popisu konektorů TGZ/TGS v češtině. Každý list odpovídá jednomu unikátnímu typu konektoru. Jelikož se často konektory v rámci TGZ opakují (typicky ty na řídicií desce), jsou zde jen jednou. Tj. Např. IO konektor 22pin weidmuller B2CF se používá pořád dokola, je zde tedy zanesen jen jednou jako „X8_IO_22pin_B2CF“</t>
   </si>
@@ -1546,6 +1550,54 @@
   </si>
   <si>
     <t xml:space="preserve">brzdný odpor 1 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Červená LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Počet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Význam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">krátké bliknutí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">podpětí Dcbus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">přepětí Dcbus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chyba fázového napětí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vysoká interní teplota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vysoká teplota softstart modulu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vysoká teplota brzdného rezistoru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rezervováno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zelená LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trvalý svit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zařízení připraveno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trvale vypnuto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zařízení nepřipraveno</t>
   </si>
 </sst>
 </file>
@@ -1705,11 +1757,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1898,8 +1950,8 @@
   </sheetPr>
   <dimension ref="A1:K178"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A136" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G170" activeCellId="0" sqref="G170"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G158" activeCellId="0" sqref="G158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11183,8 +11235,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11417,7 +11469,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11934,7 +11986,7 @@
   </sheetPr>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -14424,7 +14476,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14580,7 +14632,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14892,13 +14944,13 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N33" activeCellId="0" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
@@ -15138,6 +15190,582 @@
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="13"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>472</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I14" s="14"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="14"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I16" s="14"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I17" s="14"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I18" s="14"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I19" s="14"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,obyčejné"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,obyčejné"&amp;12Stránka &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.72"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
TGS-560-25/50 work, automation script for exporting md files from xlsx, TGZ-48-13 folder rename
</commit_message>
<xml_diff>
--- a/docs/Manual/source/tab/connectors.xlsx
+++ b/docs/Manual/source/tab/connectors.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2037" uniqueCount="492">
   <si>
     <t xml:space="preserve">Toto je sešit se zdrojovými tabulkami popisu konektorů TGZ/TGS v češtině. Každý list odpovídá jednomu unikátnímu typu konektoru. Jelikož se často konektory v rámci TGZ opakují (typicky ty na řídicií desce), jsou zde jen jednou. Tj. Např. IO konektor 22pin weidmuller B2CF se používá pořád dokola, je zde tedy zanesen jen jednou jako „X8_IO_22pin_B2CF“</t>
   </si>
@@ -1537,55 +1537,52 @@
     <t xml:space="preserve">0001</t>
   </si>
   <si>
+    <t xml:space="preserve">Zvolený 4 bit. kód</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Význam – volba funkce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">výchozí nastavení</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rezervováno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Červená LED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Počet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Význam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">krátké bliknutí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">podpětí Dcbus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">přepětí Dcbus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chyba fázového napětí</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vysoká interní teplota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vysoká teplota softstart modulu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vysoká teplota brzdného rezistoru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zelená LED</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zvolený 4 bit. kód</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Význam – volba funkce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brzdný odpor interní</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brzdný odpor 1 kW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Červená LED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Počet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Význam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">krátké bliknutí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">podpětí Dcbus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">přepětí Dcbus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chyba fázového napětí</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vysoká interní teplota</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vysoká teplota softstart modulu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vysoká teplota brzdného rezistoru</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rezervováno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zelená LED</t>
   </si>
   <si>
     <t xml:space="preserve">trvalý svit</t>
@@ -14945,7 +14942,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N33" activeCellId="0" sqref="N33"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15011,23 +15008,12 @@
         <v>471</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>472</v>
-      </c>
-    </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>473</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15035,7 +15021,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="13"/>
@@ -15045,7 +15031,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="13"/>
@@ -15055,7 +15041,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="13"/>
@@ -15065,7 +15051,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="13"/>
@@ -15075,7 +15061,7 @@
         <v>100</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="13"/>
@@ -15085,7 +15071,7 @@
         <v>101</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="13"/>
@@ -15095,7 +15081,7 @@
         <v>110</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="13"/>
@@ -15105,7 +15091,7 @@
         <v>111</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="13"/>
@@ -15115,7 +15101,7 @@
         <v>1000</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="13"/>
@@ -15125,7 +15111,7 @@
         <v>1001</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="13"/>
@@ -15135,7 +15121,7 @@
         <v>1010</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C18" s="10"/>
       <c r="H18" s="14"/>
@@ -15146,7 +15132,7 @@
         <v>1011</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="13"/>
@@ -15156,7 +15142,7 @@
         <v>1100</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H20" s="14"/>
       <c r="I20" s="13"/>
@@ -15166,7 +15152,7 @@
         <v>1101</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21" s="13"/>
@@ -15176,7 +15162,7 @@
         <v>1110</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H22" s="14"/>
       <c r="I22" s="13"/>
@@ -15186,7 +15172,7 @@
         <v>1111</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23" s="13"/>
@@ -15210,7 +15196,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15218,162 +15204,154 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
-        <v>472</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>472</v>
-      </c>
+      <c r="A10" s="13"/>
       <c r="I10" s="14"/>
       <c r="J10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>472</v>
+        <v>487</v>
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>490</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>472</v>
+        <v>487</v>
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>492</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>472</v>
+        <v>487</v>
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="13"/>
@@ -15676,10 +15654,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15714,7 +15692,7 @@
         <v>293</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>240</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15728,7 +15706,7 @@
         <v>295</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>240</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15742,7 +15720,7 @@
         <v>297</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>240</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15762,10 +15740,6 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0"/>
-      <c r="D11" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>